<commit_message>
FIX: Update xlsx test for ROUND, ROUNDUP
</commit_message>
<xml_diff>
--- a/xlsx/tests/calc_tests/ROUND.xlsx
+++ b/xlsx/tests/calc_tests/ROUND.xlsx
@@ -1,19 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC5A6DB-3AAC-4755-A290-08DB8EF75097}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EFFA00-9BDC-6C4B-A19C-B57B52ECEEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="issues" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -439,23 +451,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V40"/>
+  <dimension ref="A1:V41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -481,7 +493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.7</v>
       </c>
@@ -501,7 +513,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.7450000000000001</v>
       </c>
@@ -527,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1.7456</v>
       </c>
@@ -577,7 +589,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1.1234E-7</v>
       </c>
@@ -627,7 +639,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7.1230000000000002</v>
       </c>
@@ -653,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7.1230000000000002</v>
       </c>
@@ -673,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7.1230000000000002</v>
       </c>
@@ -693,7 +705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7.1230000000000002</v>
       </c>
@@ -713,7 +725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1234567</v>
       </c>
@@ -733,7 +745,7 @@
         <v>1234567</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1234567</v>
       </c>
@@ -753,7 +765,7 @@
         <v>1234000</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>7.1230000000000002</v>
       </c>
@@ -770,7 +782,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7.1230000000000002</v>
       </c>
@@ -790,7 +802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>3</v>
       </c>
@@ -810,7 +822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>-2.3450000000000002</v>
       </c>
@@ -830,7 +842,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>-2.3450000000000002</v>
       </c>
@@ -850,7 +862,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>-123456</v>
       </c>
@@ -870,7 +882,7 @@
         <v>-123000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
@@ -894,7 +906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>123.456</v>
       </c>
@@ -915,7 +927,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1.74499</v>
       </c>
@@ -935,7 +947,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1.745001</v>
       </c>
@@ -955,7 +967,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1.7450000000000001</v>
       </c>
@@ -972,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1.7450000000000001</v>
       </c>
@@ -995,7 +1007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1.7450000000000001</v>
       </c>
@@ -1018,7 +1030,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1.7450000000000001</v>
       </c>
@@ -1038,7 +1050,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>123456</v>
       </c>
@@ -1058,7 +1070,7 @@
         <v>123000</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>123456</v>
       </c>
@@ -1078,7 +1090,7 @@
         <v>123000</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>123456</v>
       </c>
@@ -1098,7 +1110,7 @@
         <v>123400</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>123456</v>
       </c>
@@ -1118,7 +1130,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>123456</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>123000</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>123456</v>
       </c>
@@ -1158,7 +1170,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>5</v>
       </c>
@@ -1181,7 +1193,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1.7450000000000001</v>
       </c>
@@ -1201,7 +1213,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1.7450000000000001</v>
       </c>
@@ -1221,7 +1233,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1.7450000000000001</v>
       </c>
@@ -1241,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1.7450000000000001</v>
       </c>
@@ -1261,7 +1273,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1269,19 +1281,19 @@
         <v>0</v>
       </c>
       <c r="C37" s="2" t="e">
-        <f t="shared" ref="C37:C40" si="9">ROUND(A37,B37)</f>
+        <f t="shared" ref="C37:C41" si="9">ROUND(A37,B37)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D37" s="2" t="e">
-        <f t="shared" ref="D37:D40" si="10">ROUNDUP(A37,B37)</f>
+        <f t="shared" ref="D37:D41" si="10">ROUNDUP(A37,B37)</f>
         <v>#VALUE!</v>
       </c>
       <c r="E37" s="2" t="e">
-        <f t="shared" ref="E37:E40" si="11">ROUNDDOWN(A37,B37)</f>
+        <f t="shared" ref="E37:E41" si="11">ROUNDDOWN(A37,B37)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="b">
         <v>1</v>
       </c>
@@ -1301,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="b">
         <v>0</v>
       </c>
@@ -1321,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <f>I37:I42</f>
         <v>0</v>
@@ -1340,10 +1352,55 @@
       <c r="E40" s="2">
         <f t="shared" si="11"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <f>1.05*(0.0284+0.0046)-0.0284</f>
+        <v>6.2499999999999986E-3</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="9"/>
+        <v>6.3E-3</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="10"/>
+        <v>6.3E-3</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="11"/>
+        <v>6.1999999999999998E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334FFDA0-3C7A-A242-A71C-37FEE6DF4C0A}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <f>ROUND(1.05*(0.0284+0.0046)-0.0284,4)</f>
+        <v>6.3E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>